<commit_message>
added rest of parts
</commit_message>
<xml_diff>
--- a/NodeMcu/cost and power calculations.xlsx
+++ b/NodeMcu/cost and power calculations.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>item</t>
   </si>
@@ -142,6 +142,42 @@
   </si>
   <si>
     <t>http://www.aliexpress.com/item/0603-10K-Ohm-5-1-10W-RoHS-Chip-Fixed-Resistor-SMD-Resistor-5000pcs-full-reel/32260947174.html</t>
+  </si>
+  <si>
+    <t>circuit board</t>
+  </si>
+  <si>
+    <t>3.3v regulator</t>
+  </si>
+  <si>
+    <t>http://www.aliexpress.com/item/10pcs-AMS1117-3-3-AMS1117-LM1117-1117-3-3V-1A-Voltage-Regulator/32409097011.html</t>
+  </si>
+  <si>
+    <t>micro usb connector</t>
+  </si>
+  <si>
+    <t>http://www.aliexpress.com/item/Short-term-Sacrifices-5pcs-USB-Micro-Type-B-5pin-Female-Jack-Connector-SMT-Surface-Mount/32349977492.html</t>
+  </si>
+  <si>
+    <t>micro usb cable</t>
+  </si>
+  <si>
+    <t>http://www.aliexpress.com/item/1-Meter-3-Feet-Ruggedized-Fabric-Braided-USB-Male-to-Micro-USB-Male-Data-Sync-Charging/32340270515.html</t>
+  </si>
+  <si>
+    <t>tft screen</t>
+  </si>
+  <si>
+    <t>http://www.aliexpress.com/item/Free-shipping-New-1-44-inch-LCD-color-screen-for-arduino-1-44-TFT-SPI-serial/32233128819.html</t>
+  </si>
+  <si>
+    <t>rgb led</t>
+  </si>
+  <si>
+    <t>http://www.aliexpress.com/item/1Pcs-3-Colour-RGB-SMD-LED-Board-Module-5050-Full-Color-LED-3-3-5V-for/2055617889.html</t>
+  </si>
+  <si>
+    <t>case</t>
   </si>
 </sst>
 </file>
@@ -470,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +554,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3">
-        <f t="shared" ref="B3:B8" si="0">C3*D3</f>
+        <f t="shared" ref="B3:B15" si="0">C3*D3</f>
         <v>2.2400000000000002</v>
       </c>
       <c r="C3">
@@ -622,73 +658,193 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="C9">
+        <v>0.04</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+      <c r="C10">
+        <v>0.08</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>0.72</v>
+      </c>
+      <c r="C11">
+        <v>0.72</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>3.6</v>
+      </c>
+      <c r="C12">
+        <v>3.6</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="C13">
+        <v>0.75</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>36</v>
       </c>
-      <c r="B9">
-        <f>SUM(B2:B8)</f>
-        <v>18.605</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C10">
+      <c r="B16">
+        <f>SUM(B2:B15)</f>
+        <v>33.795000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C17">
         <f>8.99/5000</f>
         <v>1.7980000000000001E-3</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E17" t="s">
         <v>37</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <f>C17*D17</f>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f>C24*D24</f>
         <v>2.4</v>
       </c>
-      <c r="C17">
+      <c r="C24">
         <v>2.4</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
         <v>28</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <f>C18*D18</f>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <f>C25*D25</f>
         <v>4.13</v>
       </c>
-      <c r="C18">
+      <c r="C25">
         <v>4.13</v>
       </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
         <v>31</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>36</v>
       </c>
-      <c r="B19">
-        <f>SUM(B17:B18)</f>
+      <c r="B26">
+        <f>SUM(B24:B25)</f>
         <v>6.5299999999999994</v>
       </c>
     </row>

</xml_diff>